<commit_message>
Premium for females implemented
</commit_message>
<xml_diff>
--- a/Resources/Selenium Assignment.xlsx
+++ b/Resources/Selenium Assignment.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t xml:space="preserve">1. Launch https://www.policybazaar.com/</t>
   </si>
@@ -255,6 +255,33 @@
   </si>
   <si>
     <t xml:space="preserve">1,830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iterm-SCN001-TC003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rina Kumari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/01/1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9874561239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Lac to 6.9 Lac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10th Pass &amp; below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">323</t>
   </si>
 </sst>
 </file>
@@ -515,7 +542,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.14"/>
   </cols>
@@ -636,10 +663,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -885,6 +912,65 @@
         <v>76</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>